<commit_message>
Add first parallel version
</commit_message>
<xml_diff>
--- a/Results/CHOLESKY_DECOMPOSITION.xlsx
+++ b/Results/CHOLESKY_DECOMPOSITION.xlsx
@@ -237,6 +237,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -250,12 +256,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3326,64 +3326,64 @@
   <dimension ref="F7:AK21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
-      <selection activeCell="Y21" sqref="Y21"/>
+      <selection activeCell="V14" sqref="V14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="7" spans="6:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="6:37" x14ac:dyDescent="0.25">
-      <c r="F8" s="25"/>
-      <c r="G8" s="20">
+      <c r="F8" s="20"/>
+      <c r="G8" s="22">
         <v>1</v>
       </c>
-      <c r="H8" s="21"/>
-      <c r="I8" s="21"/>
-      <c r="J8" s="20" t="s">
+      <c r="H8" s="23"/>
+      <c r="I8" s="23"/>
+      <c r="J8" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="K8" s="21"/>
-      <c r="L8" s="21"/>
-      <c r="M8" s="22"/>
-      <c r="N8" s="21" t="s">
+      <c r="K8" s="23"/>
+      <c r="L8" s="23"/>
+      <c r="M8" s="24"/>
+      <c r="N8" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="O8" s="21"/>
-      <c r="P8" s="21"/>
-      <c r="Q8" s="21"/>
-      <c r="R8" s="20" t="s">
+      <c r="O8" s="23"/>
+      <c r="P8" s="23"/>
+      <c r="Q8" s="23"/>
+      <c r="R8" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="S8" s="21"/>
-      <c r="T8" s="21"/>
-      <c r="U8" s="22"/>
-      <c r="V8" s="20" t="s">
+      <c r="S8" s="23"/>
+      <c r="T8" s="23"/>
+      <c r="U8" s="24"/>
+      <c r="V8" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="W8" s="21"/>
-      <c r="X8" s="21"/>
-      <c r="Y8" s="22"/>
-      <c r="Z8" s="20" t="s">
+      <c r="W8" s="23"/>
+      <c r="X8" s="23"/>
+      <c r="Y8" s="24"/>
+      <c r="Z8" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="AA8" s="21"/>
-      <c r="AB8" s="21"/>
-      <c r="AC8" s="22"/>
-      <c r="AD8" s="20" t="s">
+      <c r="AA8" s="23"/>
+      <c r="AB8" s="23"/>
+      <c r="AC8" s="24"/>
+      <c r="AD8" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="AE8" s="21"/>
-      <c r="AF8" s="21"/>
-      <c r="AG8" s="22"/>
-      <c r="AH8" s="20" t="s">
+      <c r="AE8" s="23"/>
+      <c r="AF8" s="23"/>
+      <c r="AG8" s="24"/>
+      <c r="AH8" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="AI8" s="21"/>
-      <c r="AJ8" s="21"/>
-      <c r="AK8" s="22"/>
+      <c r="AI8" s="23"/>
+      <c r="AJ8" s="23"/>
+      <c r="AK8" s="24"/>
     </row>
     <row r="9" spans="6:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F9" s="26"/>
+      <c r="F9" s="21"/>
       <c r="G9" s="1" t="s">
         <v>0</v>
       </c>
@@ -3981,7 +3981,7 @@
       <c r="AK15" s="13"/>
     </row>
     <row r="16" spans="6:37" x14ac:dyDescent="0.25">
-      <c r="F16" s="23"/>
+      <c r="F16" s="25"/>
       <c r="G16" s="17">
         <v>1</v>
       </c>
@@ -4031,7 +4031,7 @@
       <c r="AK16" s="19"/>
     </row>
     <row r="17" spans="6:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F17" s="24"/>
+      <c r="F17" s="26"/>
       <c r="G17" s="14" t="s">
         <v>0</v>
       </c>
@@ -4580,6 +4580,12 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="Z16:AC16"/>
+    <mergeCell ref="AD16:AG16"/>
+    <mergeCell ref="AH16:AK16"/>
+    <mergeCell ref="Z8:AC8"/>
+    <mergeCell ref="AD8:AG8"/>
+    <mergeCell ref="AH8:AK8"/>
     <mergeCell ref="V16:Y16"/>
     <mergeCell ref="F8:F9"/>
     <mergeCell ref="J8:M8"/>
@@ -4592,12 +4598,6 @@
     <mergeCell ref="J16:M16"/>
     <mergeCell ref="N16:Q16"/>
     <mergeCell ref="R16:U16"/>
-    <mergeCell ref="Z16:AC16"/>
-    <mergeCell ref="AD16:AG16"/>
-    <mergeCell ref="AH16:AK16"/>
-    <mergeCell ref="Z8:AC8"/>
-    <mergeCell ref="AD8:AG8"/>
-    <mergeCell ref="AH8:AK8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>